<commit_message>
Full implementation of passers. Not fully tested
</commit_message>
<xml_diff>
--- a/orobas/0x88.xlsx
+++ b/orobas/0x88.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/+Node/orobaschess/orobas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7272B6-9DF1-5F40-A07B-8C2F8E46354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E755185-D297-9945-B4F8-E0704CC8D0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-11380" windowWidth="38400" windowHeight="21140" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
+    <workbookView xWindow="25600" yWindow="-13480" windowWidth="38400" windowHeight="21140" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>turn</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>h3</t>
+  </si>
+  <si>
+    <t>Filas</t>
+  </si>
+  <si>
+    <t>Columnas</t>
   </si>
 </sst>
 </file>
@@ -606,15 +612,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD5FFF5-8CD9-3448-98D0-F4D9BE68AFF1}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10:AH17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>-5</v>
       </c>
@@ -664,7 +670,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -714,7 +720,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -764,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -814,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -864,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -914,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -964,7 +970,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1014,7 +1020,15 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="R9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1063,8 +1077,56 @@
       <c r="P10">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R10">
+        <v>7</v>
+      </c>
+      <c r="S10">
+        <v>7</v>
+      </c>
+      <c r="T10">
+        <v>7</v>
+      </c>
+      <c r="U10">
+        <v>7</v>
+      </c>
+      <c r="V10">
+        <v>7</v>
+      </c>
+      <c r="W10">
+        <v>7</v>
+      </c>
+      <c r="X10">
+        <v>7</v>
+      </c>
+      <c r="Y10">
+        <v>7</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>2</v>
+      </c>
+      <c r="AD10">
+        <v>3</v>
+      </c>
+      <c r="AE10">
+        <v>4</v>
+      </c>
+      <c r="AF10">
+        <v>5</v>
+      </c>
+      <c r="AG10">
+        <v>6</v>
+      </c>
+      <c r="AH10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
@@ -1113,8 +1175,56 @@
       <c r="P11">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R11">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <v>6</v>
+      </c>
+      <c r="T11">
+        <v>6</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+      <c r="V11">
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <v>6</v>
+      </c>
+      <c r="X11">
+        <v>6</v>
+      </c>
+      <c r="Y11">
+        <v>6</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
+        <v>3</v>
+      </c>
+      <c r="AE11">
+        <v>4</v>
+      </c>
+      <c r="AF11">
+        <v>5</v>
+      </c>
+      <c r="AG11">
+        <v>6</v>
+      </c>
+      <c r="AH11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>32</v>
       </c>
@@ -1163,8 +1273,56 @@
       <c r="P12">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R12">
+        <v>5</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <v>5</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="W12">
+        <v>5</v>
+      </c>
+      <c r="X12">
+        <v>5</v>
+      </c>
+      <c r="Y12">
+        <v>5</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>2</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AE12">
+        <v>4</v>
+      </c>
+      <c r="AF12">
+        <v>5</v>
+      </c>
+      <c r="AG12">
+        <v>6</v>
+      </c>
+      <c r="AH12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>48</v>
       </c>
@@ -1213,8 +1371,56 @@
       <c r="P13">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>4</v>
+      </c>
+      <c r="U13">
+        <v>4</v>
+      </c>
+      <c r="V13">
+        <v>4</v>
+      </c>
+      <c r="W13">
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <v>4</v>
+      </c>
+      <c r="Y13">
+        <v>4</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>2</v>
+      </c>
+      <c r="AD13">
+        <v>3</v>
+      </c>
+      <c r="AE13">
+        <v>4</v>
+      </c>
+      <c r="AF13">
+        <v>5</v>
+      </c>
+      <c r="AG13">
+        <v>6</v>
+      </c>
+      <c r="AH13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>64</v>
       </c>
@@ -1263,8 +1469,56 @@
       <c r="P14">
         <v>79</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R14">
+        <v>3</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>3</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <v>3</v>
+      </c>
+      <c r="Y14">
+        <v>3</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>2</v>
+      </c>
+      <c r="AD14">
+        <v>3</v>
+      </c>
+      <c r="AE14">
+        <v>4</v>
+      </c>
+      <c r="AF14">
+        <v>5</v>
+      </c>
+      <c r="AG14">
+        <v>6</v>
+      </c>
+      <c r="AH14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>80</v>
       </c>
@@ -1313,8 +1567,56 @@
       <c r="P15">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <v>2</v>
+      </c>
+      <c r="W15">
+        <v>2</v>
+      </c>
+      <c r="X15">
+        <v>2</v>
+      </c>
+      <c r="Y15">
+        <v>2</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>2</v>
+      </c>
+      <c r="AD15">
+        <v>3</v>
+      </c>
+      <c r="AE15">
+        <v>4</v>
+      </c>
+      <c r="AF15">
+        <v>5</v>
+      </c>
+      <c r="AG15">
+        <v>6</v>
+      </c>
+      <c r="AH15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>96</v>
       </c>
@@ -1363,8 +1665,56 @@
       <c r="P16">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>2</v>
+      </c>
+      <c r="AD16">
+        <v>3</v>
+      </c>
+      <c r="AE16">
+        <v>4</v>
+      </c>
+      <c r="AF16">
+        <v>5</v>
+      </c>
+      <c r="AG16">
+        <v>6</v>
+      </c>
+      <c r="AH16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>112</v>
       </c>
@@ -1413,8 +1763,56 @@
       <c r="P17">
         <v>127</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>2</v>
+      </c>
+      <c r="AD17">
+        <v>3</v>
+      </c>
+      <c r="AE17">
+        <v>4</v>
+      </c>
+      <c r="AF17">
+        <v>5</v>
+      </c>
+      <c r="AG17">
+        <v>6</v>
+      </c>
+      <c r="AH17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -1478,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -1591,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1626,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -1664,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Version 2.1.0 without En Passant
</commit_message>
<xml_diff>
--- a/orobas/0x88.xlsx
+++ b/orobas/0x88.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/+Node/orobaschess/orobas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202080C6-1ABB-B443-A6EA-76DD76D86648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8923AE0-1CD5-E24D-A35F-D54D1C330944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
   </bookViews>
@@ -301,10 +301,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,12 +1337,12 @@
         <v>49</v>
       </c>
       <c r="C13" s="2">
-        <v>49</v>
-      </c>
-      <c r="D13" s="7">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6">
         <v>51</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>52</v>
       </c>
       <c r="F13">
@@ -1437,10 +1437,10 @@
       <c r="C14" s="2">
         <v>66</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>67</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>68</v>
       </c>
       <c r="F14" s="1">
@@ -1872,13 +1872,13 @@
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
+      <c r="K20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
       <c r="P20" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Optimization of the evaluation function
</commit_message>
<xml_diff>
--- a/orobas/0x88.xlsx
+++ b/orobas/0x88.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/+Node/orobaschess/orobas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8923AE0-1CD5-E24D-A35F-D54D1C330944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8765811E-FFAC-5243-96BE-815A174A0162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" activeTab="1" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="0x88" sheetId="1" r:id="rId1"/>
+    <sheet name="KingRaysAttack" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -235,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,8 +250,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +290,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -288,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -305,6 +332,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD5FFF5-8CD9-3448-98D0-F4D9BE68AFF1}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2129,4 +2161,833 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242DE764-237B-9F4D-B0C2-1E3220C42431}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16" width="4.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10">
+        <v>11</v>
+      </c>
+      <c r="M1" s="10">
+        <v>12</v>
+      </c>
+      <c r="N1" s="10">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8">
+        <v>18</v>
+      </c>
+      <c r="D2" s="8">
+        <v>19</v>
+      </c>
+      <c r="E2" s="8">
+        <v>20</v>
+      </c>
+      <c r="F2" s="8">
+        <v>21</v>
+      </c>
+      <c r="G2" s="12">
+        <v>22</v>
+      </c>
+      <c r="H2" s="8">
+        <v>23</v>
+      </c>
+      <c r="I2" s="10">
+        <v>24</v>
+      </c>
+      <c r="J2" s="10">
+        <v>25</v>
+      </c>
+      <c r="K2" s="10">
+        <v>26</v>
+      </c>
+      <c r="L2" s="10">
+        <v>27</v>
+      </c>
+      <c r="M2" s="10">
+        <v>28</v>
+      </c>
+      <c r="N2" s="10">
+        <v>29</v>
+      </c>
+      <c r="O2" s="10">
+        <v>30</v>
+      </c>
+      <c r="P2" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>32</v>
+      </c>
+      <c r="B3" s="12">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8">
+        <v>34</v>
+      </c>
+      <c r="D3" s="8">
+        <v>35</v>
+      </c>
+      <c r="E3" s="8">
+        <v>36</v>
+      </c>
+      <c r="F3" s="8">
+        <v>37</v>
+      </c>
+      <c r="G3" s="12">
+        <v>38</v>
+      </c>
+      <c r="H3" s="8">
+        <v>39</v>
+      </c>
+      <c r="I3" s="10">
+        <v>40</v>
+      </c>
+      <c r="J3" s="10">
+        <v>41</v>
+      </c>
+      <c r="K3" s="10">
+        <v>42</v>
+      </c>
+      <c r="L3" s="10">
+        <v>43</v>
+      </c>
+      <c r="M3" s="10">
+        <v>44</v>
+      </c>
+      <c r="N3" s="10">
+        <v>45</v>
+      </c>
+      <c r="O3" s="10">
+        <v>46</v>
+      </c>
+      <c r="P3" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12">
+        <v>50</v>
+      </c>
+      <c r="D4" s="8">
+        <v>51</v>
+      </c>
+      <c r="E4" s="8">
+        <v>52</v>
+      </c>
+      <c r="F4" s="8">
+        <v>53</v>
+      </c>
+      <c r="G4" s="12">
+        <v>54</v>
+      </c>
+      <c r="H4" s="8">
+        <v>55</v>
+      </c>
+      <c r="I4" s="10">
+        <v>56</v>
+      </c>
+      <c r="J4" s="10">
+        <v>57</v>
+      </c>
+      <c r="K4" s="10">
+        <v>58</v>
+      </c>
+      <c r="L4" s="10">
+        <v>59</v>
+      </c>
+      <c r="M4" s="10">
+        <v>60</v>
+      </c>
+      <c r="N4" s="10">
+        <v>61</v>
+      </c>
+      <c r="O4" s="10">
+        <v>62</v>
+      </c>
+      <c r="P4" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8">
+        <v>65</v>
+      </c>
+      <c r="C5" s="8">
+        <v>66</v>
+      </c>
+      <c r="D5" s="12">
+        <v>67</v>
+      </c>
+      <c r="E5" s="8">
+        <v>68</v>
+      </c>
+      <c r="F5" s="8">
+        <v>69</v>
+      </c>
+      <c r="G5" s="12">
+        <v>70</v>
+      </c>
+      <c r="H5" s="8">
+        <v>71</v>
+      </c>
+      <c r="I5" s="10">
+        <v>72</v>
+      </c>
+      <c r="J5" s="10">
+        <v>73</v>
+      </c>
+      <c r="K5" s="10">
+        <v>74</v>
+      </c>
+      <c r="L5" s="10">
+        <v>75</v>
+      </c>
+      <c r="M5" s="10">
+        <v>76</v>
+      </c>
+      <c r="N5" s="10">
+        <v>77</v>
+      </c>
+      <c r="O5" s="10">
+        <v>78</v>
+      </c>
+      <c r="P5" s="10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>80</v>
+      </c>
+      <c r="B6" s="8">
+        <v>81</v>
+      </c>
+      <c r="C6" s="8">
+        <v>82</v>
+      </c>
+      <c r="D6" s="8">
+        <v>83</v>
+      </c>
+      <c r="E6" s="12">
+        <v>84</v>
+      </c>
+      <c r="F6" s="8">
+        <v>85</v>
+      </c>
+      <c r="G6" s="12">
+        <v>86</v>
+      </c>
+      <c r="H6" s="8">
+        <v>87</v>
+      </c>
+      <c r="I6" s="10">
+        <v>88</v>
+      </c>
+      <c r="J6" s="10">
+        <v>89</v>
+      </c>
+      <c r="K6" s="10">
+        <v>90</v>
+      </c>
+      <c r="L6" s="10">
+        <v>91</v>
+      </c>
+      <c r="M6" s="10">
+        <v>92</v>
+      </c>
+      <c r="N6" s="10">
+        <v>93</v>
+      </c>
+      <c r="O6" s="10">
+        <v>94</v>
+      </c>
+      <c r="P6" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>96</v>
+      </c>
+      <c r="B7" s="8">
+        <v>97</v>
+      </c>
+      <c r="C7" s="8">
+        <v>98</v>
+      </c>
+      <c r="D7" s="8">
+        <v>99</v>
+      </c>
+      <c r="E7" s="8">
+        <v>100</v>
+      </c>
+      <c r="F7" s="12">
+        <v>101</v>
+      </c>
+      <c r="G7" s="12">
+        <v>102</v>
+      </c>
+      <c r="H7" s="12">
+        <v>103</v>
+      </c>
+      <c r="I7" s="10">
+        <v>104</v>
+      </c>
+      <c r="J7" s="10">
+        <v>105</v>
+      </c>
+      <c r="K7" s="10">
+        <v>106</v>
+      </c>
+      <c r="L7" s="10">
+        <v>107</v>
+      </c>
+      <c r="M7" s="10">
+        <v>108</v>
+      </c>
+      <c r="N7" s="10">
+        <v>109</v>
+      </c>
+      <c r="O7" s="10">
+        <v>110</v>
+      </c>
+      <c r="P7" s="10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>112</v>
+      </c>
+      <c r="B8" s="12">
+        <v>113</v>
+      </c>
+      <c r="C8" s="12">
+        <v>114</v>
+      </c>
+      <c r="D8" s="12">
+        <v>115</v>
+      </c>
+      <c r="E8" s="12">
+        <v>116</v>
+      </c>
+      <c r="F8" s="12">
+        <v>117</v>
+      </c>
+      <c r="G8" s="11">
+        <v>118</v>
+      </c>
+      <c r="H8" s="12">
+        <v>119</v>
+      </c>
+      <c r="I8" s="10">
+        <v>120</v>
+      </c>
+      <c r="J8" s="10">
+        <v>121</v>
+      </c>
+      <c r="K8" s="10">
+        <v>122</v>
+      </c>
+      <c r="L8" s="10">
+        <v>123</v>
+      </c>
+      <c r="M8" s="10">
+        <v>124</v>
+      </c>
+      <c r="N8" s="10">
+        <v>125</v>
+      </c>
+      <c r="O8" s="10">
+        <v>126</v>
+      </c>
+      <c r="P8" s="10">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>0</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8">
+        <v>6</v>
+      </c>
+      <c r="H10" s="8">
+        <v>7</v>
+      </c>
+      <c r="I10" s="10">
+        <v>8</v>
+      </c>
+      <c r="J10" s="10">
+        <v>9</v>
+      </c>
+      <c r="K10" s="10">
+        <v>10</v>
+      </c>
+      <c r="L10" s="10">
+        <v>11</v>
+      </c>
+      <c r="M10" s="10">
+        <v>12</v>
+      </c>
+      <c r="N10" s="10">
+        <v>13</v>
+      </c>
+      <c r="O10" s="10">
+        <v>14</v>
+      </c>
+      <c r="P10" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>16</v>
+      </c>
+      <c r="B11" s="8">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8">
+        <v>19</v>
+      </c>
+      <c r="E11" s="8">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8">
+        <v>21</v>
+      </c>
+      <c r="G11" s="8">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8">
+        <v>23</v>
+      </c>
+      <c r="I11" s="10">
+        <v>24</v>
+      </c>
+      <c r="J11" s="10">
+        <v>25</v>
+      </c>
+      <c r="K11" s="10">
+        <v>26</v>
+      </c>
+      <c r="L11" s="10">
+        <v>27</v>
+      </c>
+      <c r="M11" s="10">
+        <v>28</v>
+      </c>
+      <c r="N11" s="10">
+        <v>29</v>
+      </c>
+      <c r="O11" s="10">
+        <v>30</v>
+      </c>
+      <c r="P11" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>32</v>
+      </c>
+      <c r="B12" s="8">
+        <v>33</v>
+      </c>
+      <c r="C12" s="8">
+        <v>34</v>
+      </c>
+      <c r="D12" s="8">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8">
+        <v>36</v>
+      </c>
+      <c r="F12" s="8">
+        <v>37</v>
+      </c>
+      <c r="G12" s="8">
+        <v>38</v>
+      </c>
+      <c r="H12" s="8">
+        <v>39</v>
+      </c>
+      <c r="I12" s="10">
+        <v>40</v>
+      </c>
+      <c r="J12" s="10">
+        <v>41</v>
+      </c>
+      <c r="K12" s="10">
+        <v>42</v>
+      </c>
+      <c r="L12" s="10">
+        <v>43</v>
+      </c>
+      <c r="M12" s="10">
+        <v>44</v>
+      </c>
+      <c r="N12" s="10">
+        <v>45</v>
+      </c>
+      <c r="O12" s="10">
+        <v>46</v>
+      </c>
+      <c r="P12" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>48</v>
+      </c>
+      <c r="B13" s="8">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8">
+        <v>50</v>
+      </c>
+      <c r="D13" s="8">
+        <v>51</v>
+      </c>
+      <c r="E13" s="8">
+        <v>52</v>
+      </c>
+      <c r="F13" s="8">
+        <v>53</v>
+      </c>
+      <c r="G13" s="8">
+        <v>54</v>
+      </c>
+      <c r="H13" s="8">
+        <v>55</v>
+      </c>
+      <c r="I13" s="10">
+        <v>56</v>
+      </c>
+      <c r="J13" s="10">
+        <v>57</v>
+      </c>
+      <c r="K13" s="10">
+        <v>58</v>
+      </c>
+      <c r="L13" s="10">
+        <v>59</v>
+      </c>
+      <c r="M13" s="10">
+        <v>60</v>
+      </c>
+      <c r="N13" s="10">
+        <v>61</v>
+      </c>
+      <c r="O13" s="10">
+        <v>62</v>
+      </c>
+      <c r="P13" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>64</v>
+      </c>
+      <c r="B14" s="8">
+        <v>65</v>
+      </c>
+      <c r="C14" s="8">
+        <v>66</v>
+      </c>
+      <c r="D14" s="8">
+        <v>67</v>
+      </c>
+      <c r="E14" s="8">
+        <v>68</v>
+      </c>
+      <c r="F14" s="8">
+        <v>69</v>
+      </c>
+      <c r="G14" s="8">
+        <v>70</v>
+      </c>
+      <c r="H14" s="8">
+        <v>71</v>
+      </c>
+      <c r="I14" s="10">
+        <v>72</v>
+      </c>
+      <c r="J14" s="10">
+        <v>73</v>
+      </c>
+      <c r="K14" s="10">
+        <v>74</v>
+      </c>
+      <c r="L14" s="10">
+        <v>75</v>
+      </c>
+      <c r="M14" s="10">
+        <v>76</v>
+      </c>
+      <c r="N14" s="10">
+        <v>77</v>
+      </c>
+      <c r="O14" s="10">
+        <v>78</v>
+      </c>
+      <c r="P14" s="10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>80</v>
+      </c>
+      <c r="B15" s="8">
+        <v>81</v>
+      </c>
+      <c r="C15" s="8">
+        <v>82</v>
+      </c>
+      <c r="D15" s="8">
+        <v>83</v>
+      </c>
+      <c r="E15" s="8">
+        <v>84</v>
+      </c>
+      <c r="F15" s="8">
+        <v>85</v>
+      </c>
+      <c r="G15" s="8">
+        <v>86</v>
+      </c>
+      <c r="H15" s="8">
+        <v>87</v>
+      </c>
+      <c r="I15" s="10">
+        <v>88</v>
+      </c>
+      <c r="J15" s="10">
+        <v>89</v>
+      </c>
+      <c r="K15" s="10">
+        <v>90</v>
+      </c>
+      <c r="L15" s="10">
+        <v>91</v>
+      </c>
+      <c r="M15" s="10">
+        <v>92</v>
+      </c>
+      <c r="N15" s="10">
+        <v>93</v>
+      </c>
+      <c r="O15" s="10">
+        <v>94</v>
+      </c>
+      <c r="P15" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>96</v>
+      </c>
+      <c r="B16" s="8">
+        <v>97</v>
+      </c>
+      <c r="C16" s="8">
+        <v>98</v>
+      </c>
+      <c r="D16" s="8">
+        <v>99</v>
+      </c>
+      <c r="E16" s="8">
+        <v>100</v>
+      </c>
+      <c r="F16" s="8">
+        <v>101</v>
+      </c>
+      <c r="G16" s="8">
+        <v>102</v>
+      </c>
+      <c r="H16" s="8">
+        <v>103</v>
+      </c>
+      <c r="I16" s="10">
+        <v>104</v>
+      </c>
+      <c r="J16" s="10">
+        <v>105</v>
+      </c>
+      <c r="K16" s="10">
+        <v>106</v>
+      </c>
+      <c r="L16" s="10">
+        <v>107</v>
+      </c>
+      <c r="M16" s="10">
+        <v>108</v>
+      </c>
+      <c r="N16" s="10">
+        <v>109</v>
+      </c>
+      <c r="O16" s="10">
+        <v>110</v>
+      </c>
+      <c r="P16" s="10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>112</v>
+      </c>
+      <c r="B17" s="8">
+        <v>113</v>
+      </c>
+      <c r="C17" s="8">
+        <v>114</v>
+      </c>
+      <c r="D17" s="8">
+        <v>115</v>
+      </c>
+      <c r="E17" s="8">
+        <v>116</v>
+      </c>
+      <c r="F17" s="8">
+        <v>117</v>
+      </c>
+      <c r="G17" s="8">
+        <v>118</v>
+      </c>
+      <c r="H17" s="8">
+        <v>119</v>
+      </c>
+      <c r="I17" s="10">
+        <v>120</v>
+      </c>
+      <c r="J17" s="10">
+        <v>121</v>
+      </c>
+      <c r="K17" s="10">
+        <v>122</v>
+      </c>
+      <c r="L17" s="10">
+        <v>123</v>
+      </c>
+      <c r="M17" s="10">
+        <v>124</v>
+      </c>
+      <c r="N17" s="10">
+        <v>125</v>
+      </c>
+      <c r="O17" s="10">
+        <v>126</v>
+      </c>
+      <c r="P17" s="10">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Optimization of history heuristic. Not fully tested
</commit_message>
<xml_diff>
--- a/orobas/0x88.xlsx
+++ b/orobas/0x88.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/+Node/orobaschess/orobas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8765811E-FFAC-5243-96BE-815A174A0162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F80CE-E9D2-7041-8542-E1AE9729C94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" activeTab="1" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
   </bookViews>
   <sheets>
     <sheet name="0x88" sheetId="1" r:id="rId1"/>
-    <sheet name="KingRaysAttack" sheetId="2" r:id="rId2"/>
+    <sheet name="Diagonals" sheetId="3" r:id="rId2"/>
+    <sheet name="KingRaysAttack" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="69">
   <si>
     <t>turn</t>
   </si>
@@ -230,6 +231,9 @@
   </si>
   <si>
     <t>Columnas</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -265,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +306,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -315,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -329,14 +339,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1904,13 +1915,13 @@
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
+      <c r="K20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
       <c r="P20" s="3" t="s">
         <v>0</v>
       </c>
@@ -2164,826 +2175,2231 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402B31B9-C341-344F-ABAE-E2365C8CE01E}">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="13">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13">
+        <f>A2</f>
+        <v>1</v>
+      </c>
+      <c r="C1" s="13">
+        <f t="shared" ref="C1:H17" si="0">B2</f>
+        <v>2</v>
+      </c>
+      <c r="D1" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E1" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F1" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G1" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H1" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13">
+        <f t="shared" ref="B2:H18" si="1">A3</f>
+        <v>2</v>
+      </c>
+      <c r="C2" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D2" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E2" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F2" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G2" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H2" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C3" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C4" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="13">
+        <f t="shared" ref="A17:G31" si="2">B18</f>
+        <v>7</v>
+      </c>
+      <c r="B17" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="C17" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D17" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <f>H18</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B18" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D18" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G18" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B19" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G19" s="13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H19" s="13">
+        <v>2</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D20" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G20" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H20" s="13">
+        <v>3</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B21" s="13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="C21" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D21" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G21" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H21" s="13">
+        <v>4</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B22" s="13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C22" s="13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D22" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G22" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="H22" s="13">
+        <v>5</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="13">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B23" s="13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="C23" s="13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D23" s="13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G23" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="H23" s="13">
+        <v>6</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P23" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="13">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B24" s="13">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="C24" s="13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D24" s="13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G24" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H24" s="13">
+        <v>7</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B25" s="8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="C25" s="8">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D25" s="8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="H25" s="8">
+        <v>8</v>
+      </c>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B26" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C26" s="8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H26" s="8">
+        <v>9</v>
+      </c>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B27" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C27" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="H27" s="8">
+        <v>10</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B28" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C28" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H28" s="8">
+        <v>11</v>
+      </c>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B29" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C29" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="H29" s="8">
+        <v>12</v>
+      </c>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="H30" s="8">
+        <v>13</v>
+      </c>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="B31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
+        <v>14</v>
+      </c>
+      <c r="I31" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242DE764-237B-9F4D-B0C2-1E3220C42431}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16" width="4.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="16" width="4.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="8">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8">
+      <c r="A1" s="7">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7">
         <v>2</v>
       </c>
-      <c r="D1" s="8">
+      <c r="D1" s="7">
         <v>3</v>
       </c>
-      <c r="E1" s="8">
+      <c r="E1" s="7">
         <v>4</v>
       </c>
-      <c r="F1" s="8">
+      <c r="F1" s="7">
         <v>5</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="11">
         <v>6</v>
       </c>
-      <c r="H1" s="8">
+      <c r="H1" s="7">
         <v>7</v>
       </c>
-      <c r="I1" s="10">
+      <c r="I1" s="9">
         <v>8</v>
       </c>
-      <c r="J1" s="10">
+      <c r="J1" s="9">
         <v>9</v>
       </c>
-      <c r="K1" s="10">
+      <c r="K1" s="9">
         <v>10</v>
       </c>
-      <c r="L1" s="10">
+      <c r="L1" s="9">
         <v>11</v>
       </c>
-      <c r="M1" s="10">
+      <c r="M1" s="9">
         <v>12</v>
       </c>
-      <c r="N1" s="10">
+      <c r="N1" s="9">
         <v>13</v>
       </c>
-      <c r="O1" s="10">
+      <c r="O1" s="9">
         <v>14</v>
       </c>
-      <c r="P1" s="10">
+      <c r="P1" s="9">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>16</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>17</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>18</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>19</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>20</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>21</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <v>22</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>23</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="9">
         <v>24</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>25</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="9">
         <v>26</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="9">
         <v>27</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <v>28</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="9">
         <v>29</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="9">
         <v>30</v>
       </c>
-      <c r="P2" s="10">
+      <c r="P2" s="9">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>32</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>33</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>34</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>35</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>36</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>37</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>38</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>39</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <v>40</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>41</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>42</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <v>43</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <v>44</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>45</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9">
         <v>46</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="9">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>48</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>49</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>50</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>51</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>52</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>53</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>54</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>55</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>56</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>57</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>58</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>59</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>60</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <v>61</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <v>62</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="9">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>64</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>65</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>66</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>67</v>
       </c>
-      <c r="E5" s="8">
-        <v>68</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="E5" s="7">
+        <v>68</v>
+      </c>
+      <c r="F5" s="7">
         <v>69</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>70</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>71</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>72</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>73</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>74</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="9">
         <v>75</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>76</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <v>77</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>78</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="9">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>80</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>81</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>82</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>83</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>84</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>85</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11">
         <v>86</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>87</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>88</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>89</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>90</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>91</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>92</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <v>93</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>94</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="9">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>96</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>97</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>98</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>99</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>100</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>101</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>102</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>103</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>104</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>105</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>106</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="9">
         <v>107</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <v>108</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <v>109</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>110</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="9">
         <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>112</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>113</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>114</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>115</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>116</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>117</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>118</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>119</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>120</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>121</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>122</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <v>123</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <v>124</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <v>125</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>126</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="9">
         <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>0</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="A10" s="7">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
         <v>2</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>3</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>4</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>5</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>6</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>7</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>8</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>9</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>10</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <v>11</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>12</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="9">
         <v>13</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>14</v>
       </c>
-      <c r="P10" s="10">
+      <c r="P10" s="9">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>16</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>17</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>18</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>19</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>20</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>21</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>22</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>23</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>24</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>25</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>26</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <v>27</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>28</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="9">
         <v>29</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>30</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="9">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>32</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>33</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>34</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>35</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>36</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>37</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>38</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>39</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>40</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>41</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>42</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <v>43</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="9">
         <v>44</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="9">
         <v>45</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>46</v>
       </c>
-      <c r="P12" s="10">
+      <c r="P12" s="9">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>48</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>49</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>50</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>51</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>52</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>53</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>54</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>55</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>56</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>57</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>58</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="9">
         <v>59</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <v>60</v>
       </c>
-      <c r="N13" s="10">
+      <c r="N13" s="9">
         <v>61</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>62</v>
       </c>
-      <c r="P13" s="10">
+      <c r="P13" s="9">
         <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>64</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>65</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>66</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>67</v>
       </c>
-      <c r="E14" s="8">
-        <v>68</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E14" s="7">
+        <v>68</v>
+      </c>
+      <c r="F14" s="7">
         <v>69</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>70</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>71</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>72</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>73</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>74</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <v>75</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <v>76</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="9">
         <v>77</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>78</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="9">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>80</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>81</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>82</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>83</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>84</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>85</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>86</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <v>87</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <v>88</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>89</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <v>90</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="9">
         <v>91</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>92</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="9">
         <v>93</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9">
         <v>94</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="9">
         <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>96</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>97</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>98</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>99</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>100</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>101</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>102</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>103</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <v>104</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="9">
         <v>105</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="9">
         <v>106</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="9">
         <v>107</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <v>108</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="9">
         <v>109</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9">
         <v>110</v>
       </c>
-      <c r="P16" s="10">
+      <c r="P16" s="9">
         <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>112</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>113</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>114</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>115</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>116</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>117</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>118</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <v>119</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>120</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
         <v>121</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="9">
         <v>122</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="9">
         <v>123</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="9">
         <v>124</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="9">
         <v>125</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="9">
         <v>126</v>
       </c>
-      <c r="P17" s="10">
+      <c r="P17" s="9">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved version with all modifications made in OrobasUI. +124 ELO
</commit_message>
<xml_diff>
--- a/orobas/0x88.xlsx
+++ b/orobas/0x88.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/+Node/orobaschess/orobas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F80CE-E9D2-7041-8542-E1AE9729C94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F12A318-C89C-1A4B-A84C-631CBFA9620E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" activeTab="1" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{CD1183D7-23ED-334D-923D-1AFE388EA7B4}"/>
   </bookViews>
   <sheets>
     <sheet name="0x88" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -344,10 +351,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD5FFF5-8CD9-3448-98D0-F4D9BE68AFF1}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1915,13 +1922,13 @@
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
+      <c r="K20" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
       <c r="P20" s="3" t="s">
         <v>0</v>
       </c>
@@ -2178,465 +2185,465 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402B31B9-C341-344F-ABAE-E2365C8CE01E}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="13">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13">
+      <c r="A1" s="12">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12">
         <f>A2</f>
         <v>1</v>
       </c>
-      <c r="C1" s="13">
-        <f t="shared" ref="C1:H17" si="0">B2</f>
+      <c r="C1" s="12">
+        <f t="shared" ref="C1:H15" si="0">B2</f>
         <v>2</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F1" s="13">
+      <c r="F1" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G1" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P1" s="13" t="s">
+      <c r="I1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13">
-        <f t="shared" ref="B2:H18" si="1">A3</f>
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <f t="shared" ref="B2:G15" si="1">A3</f>
         <v>2</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="I2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P3" s="13" t="s">
+      <c r="I3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P4" s="13" t="s">
+      <c r="I4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P5" s="13" t="s">
+      <c r="I5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P6" s="13" t="s">
+      <c r="I6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P7" s="13" t="s">
+      <c r="I7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P8" s="13" t="s">
+      <c r="I8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2668,7 +2675,7 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2701,7 +2708,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2734,7 +2741,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2767,7 +2774,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2800,7 +2807,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2833,7 +2840,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2866,7 +2873,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2881,458 +2888,458 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="13">
+      <c r="A17" s="12">
         <f t="shared" ref="A17:G31" si="2">B18</f>
         <v>7</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="12">
         <f>H18</f>
         <v>1</v>
       </c>
-      <c r="H17" s="13">
-        <v>0</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O17" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P17" s="13" t="s">
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="13">
+      <c r="A18" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H18" s="13">
-        <v>1</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O18" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P18" s="13" t="s">
+      <c r="H18" s="12">
+        <v>1</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
+      <c r="A19" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="12">
         <v>2</v>
       </c>
-      <c r="I19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P19" s="13" t="s">
+      <c r="I19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
+      <c r="A20" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="12">
         <v>3</v>
       </c>
-      <c r="I20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P20" s="13" t="s">
+      <c r="I20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="13">
+      <c r="A21" s="12">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <v>4</v>
       </c>
-      <c r="I21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P21" s="13" t="s">
+      <c r="I21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P21" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
+      <c r="A22" s="12">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="12">
         <v>5</v>
       </c>
-      <c r="I22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O22" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P22" s="13" t="s">
+      <c r="I22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P22" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
+      <c r="A23" s="12">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="12">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="12">
         <v>6</v>
       </c>
-      <c r="I23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P23" s="13" t="s">
+      <c r="I23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P23" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+      <c r="A24" s="12">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="12">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="12">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="12">
         <v>7</v>
       </c>
-      <c r="I24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="P24" s="13" t="s">
+      <c r="I24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P24" s="12" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>